<commit_message>
file added for 8/22)
</commit_message>
<xml_diff>
--- a/document/Git使用方法.xlsx
+++ b/document/Git使用方法.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18315" windowHeight="8490" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18315" windowHeight="8490" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Git_GitHubとは" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="244">
   <si>
     <t>ブラウザで以下のURLを開く。</t>
     <rPh sb="5" eb="7">
@@ -1893,6 +1893,107 @@
     </rPh>
     <rPh sb="26" eb="27">
       <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>merge fast-forward</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>merge non-fast-forward</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>分岐前の元ブランチが更新されていない場合、新しいブランチと元ブランチを一本にして(分岐がなかったことになる)マージする</t>
+    <rPh sb="0" eb="2">
+      <t>ブンキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>イッポン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ブンキ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>分岐前のブランチが更新されていなくても、新しいブランチを作成した履歴を残してマージする</t>
+    <rPh sb="0" eb="2">
+      <t>ブンキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>リレキ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>ノコ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rebase</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>すべて一本のブランチで作業したようにマージする</t>
+    <rPh sb="3" eb="5">
+      <t>イッポン</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サギョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rebaseの利用例</t>
+    <rPh sb="7" eb="9">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.backlog.jp/git-guide/stepup/stepup1_5.html</t>
+  </si>
+  <si>
+    <t>http://keijinsonyaban.blogspot.jp/2010/10/successful-git-branching-model.html</t>
+  </si>
+  <si>
+    <t>ブランチのモデル例</t>
+    <rPh sb="8" eb="9">
+      <t>レイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -4987,7 +5088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -5409,10 +5510,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:J42"/>
+  <dimension ref="B3:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5565,29 +5666,63 @@
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:11">
       <c r="B36" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="37" spans="2:3">
+      <c r="I36" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="J36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
       <c r="C37" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="39" spans="2:3">
+      <c r="I37" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="J37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="I38" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J38" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
       <c r="C39" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="41" spans="2:3">
+      <c r="J39" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="K40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
       <c r="B41" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="42" spans="2:3">
+      <c r="J41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
       <c r="B42" t="s">
         <v>214</v>
+      </c>
+      <c r="K42" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>